<commit_message>
:fire: working in commercial slide for pbi executive
</commit_message>
<xml_diff>
--- a/src/b4d_pbi_executive_dashboard/src/b4d_abril.xlsx
+++ b/src/b4d_pbi_executive_dashboard/src/b4d_abril.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\b4d\data\raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\b4d\projects\b4d_analytics\src\b4d_pbi_executive_dashboard\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{364FA2CE-9919-4D21-B161-E66E54FADEC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F9853B8-F1B3-45DB-9F69-2367E5B2B79E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9405" yWindow="5055" windowWidth="15360" windowHeight="7350" xr2:uid="{586F4F54-FFF4-4F9F-87C4-B95A1BF10EA3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{586F4F54-FFF4-4F9F-87C4-B95A1BF10EA3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -189,9 +189,6 @@
     <t>868dkv507</t>
   </si>
   <si>
-    <t>BANCO ECOFUTURO CAMPAÃ‘AS</t>
-  </si>
-  <si>
     <t>868dkuzv6</t>
   </si>
   <si>
@@ -219,9 +216,6 @@
     <t>868df7mj1</t>
   </si>
   <si>
-    <t>CEPA - CÃMARAS</t>
-  </si>
-  <si>
     <t>El Salvador</t>
   </si>
   <si>
@@ -240,9 +234,6 @@
     <t>868cvmd6y</t>
   </si>
   <si>
-    <t>AVICOLA SALVADOREÃ‘A</t>
-  </si>
-  <si>
     <t>New Sell</t>
   </si>
   <si>
@@ -534,9 +525,6 @@
     <t>868df99r5</t>
   </si>
   <si>
-    <t>SOBOCE - CÃMARAS</t>
-  </si>
-  <si>
     <t>868cuugtx</t>
   </si>
   <si>
@@ -612,9 +600,6 @@
     <t>868det13a</t>
   </si>
   <si>
-    <t>TIGO LICITACIÃ“N B2B</t>
-  </si>
-  <si>
     <t>868daa7wf</t>
   </si>
   <si>
@@ -624,9 +609,6 @@
     <t>868da9qeb</t>
   </si>
   <si>
-    <t>HAKA CÃMARA GACIP</t>
-  </si>
-  <si>
     <t>HAKA TECHNOLOGIES</t>
   </si>
   <si>
@@ -714,9 +696,6 @@
     <t>868bqac09</t>
   </si>
   <si>
-    <t>EMBOL (CLASIFICACIÃ“N DE CANALES)</t>
-  </si>
-  <si>
     <t>["Franz Claure"]</t>
   </si>
   <si>
@@ -1003,6 +982,27 @@
   </si>
   <si>
     <t>TIGO EL SALVADOR</t>
+  </si>
+  <si>
+    <t>BANCO ECOFUTURO CAMPAÑAS</t>
+  </si>
+  <si>
+    <t>EMBOL (CLASIFICACIÓN DE CANALES)</t>
+  </si>
+  <si>
+    <t>HAKA CÁMARA GACIP</t>
+  </si>
+  <si>
+    <t>SOBOCE - CÁMARAS</t>
+  </si>
+  <si>
+    <t>TIGO LICITACIÓN B2B</t>
+  </si>
+  <si>
+    <t>CEPA - CÁMARAS</t>
+  </si>
+  <si>
+    <t>AVICOLA SALVADOREÑA</t>
   </si>
 </sst>
 </file>
@@ -1364,8 +1364,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBF7A4E2-C5FA-4E23-A9FB-89BEEDC87861}">
   <dimension ref="A1:AD81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:XFD18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1375,6 +1375,7 @@
     <col min="9" max="9" width="30.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="11.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="27" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="10.85546875" customWidth="1"/>
     <col min="24" max="24" width="19" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="32" bestFit="1" customWidth="1"/>
@@ -1470,7 +1471,7 @@
         <v>27</v>
       </c>
       <c r="AC1" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="AD1" t="s">
         <v>28</v>
@@ -1487,14 +1488,14 @@
         <v>45790</v>
       </c>
       <c r="D2" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="G2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="I2" t="s">
         <v>41</v>
@@ -1506,13 +1507,13 @@
         <v>824770</v>
       </c>
       <c r="M2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="N2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="O2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="P2" t="s">
         <v>37</v>
@@ -1530,13 +1531,13 @@
         <v>90113131698</v>
       </c>
       <c r="AA2" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="AB2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="AC2" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.25">
@@ -1550,14 +1551,14 @@
         <v>45790</v>
       </c>
       <c r="D3" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="G3" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="I3" t="s">
         <v>31</v>
@@ -1566,16 +1567,16 @@
         <v>6200</v>
       </c>
       <c r="M3" t="s">
+        <v>59</v>
+      </c>
+      <c r="N3" t="s">
         <v>60</v>
       </c>
-      <c r="N3" t="s">
-        <v>61</v>
-      </c>
       <c r="O3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="P3" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="Q3" t="s">
         <v>38</v>
@@ -1593,13 +1594,13 @@
         <v>45805</v>
       </c>
       <c r="AA3" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="AB3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="AC3" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.25">
@@ -1613,23 +1614,23 @@
         <v>45790</v>
       </c>
       <c r="D4" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="G4" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="I4" t="s">
         <v>41</v>
       </c>
       <c r="M4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="N4" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="P4" t="s">
         <v>37</v>
@@ -1644,7 +1645,7 @@
         <v>36</v>
       </c>
       <c r="AC4" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.25">
@@ -1658,29 +1659,29 @@
         <v>45790</v>
       </c>
       <c r="D5" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G5" t="s">
-        <v>70</v>
+        <v>324</v>
       </c>
       <c r="I5" t="s">
         <v>41</v>
       </c>
       <c r="M5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="N5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="O5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="P5" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="V5" s="1">
         <v>45716</v>
@@ -1692,13 +1693,13 @@
         <v>90113131698</v>
       </c>
       <c r="AA5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="AB5" t="s">
         <v>36</v>
       </c>
       <c r="AC5" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
@@ -1712,14 +1713,14 @@
         <v>45790</v>
       </c>
       <c r="D6" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="G6" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="I6" t="s">
         <v>31</v>
@@ -1728,10 +1729,10 @@
         <v>50000</v>
       </c>
       <c r="M6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="O6" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="P6" t="s">
         <v>37</v>
@@ -1749,13 +1750,13 @@
         <v>45761</v>
       </c>
       <c r="AA6" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="AB6" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="AC6" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.25">
@@ -1769,14 +1770,14 @@
         <v>45790</v>
       </c>
       <c r="D7" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G7" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="I7" t="s">
         <v>31</v>
@@ -1794,13 +1795,13 @@
         <v>90113131698</v>
       </c>
       <c r="AA7" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="AB7" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="AC7" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.25">
@@ -1814,14 +1815,14 @@
         <v>45790</v>
       </c>
       <c r="D8" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="G8" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="I8" t="s">
         <v>31</v>
@@ -1833,16 +1834,16 @@
         <v>6500</v>
       </c>
       <c r="M8" t="s">
+        <v>59</v>
+      </c>
+      <c r="N8" t="s">
         <v>60</v>
       </c>
-      <c r="N8" t="s">
-        <v>61</v>
-      </c>
       <c r="O8" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="P8" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="Q8" t="s">
         <v>38</v>
@@ -1860,13 +1861,13 @@
         <v>45799</v>
       </c>
       <c r="AA8" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="AB8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="AC8" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.25">
@@ -1880,23 +1881,23 @@
         <v>45790</v>
       </c>
       <c r="D9" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="G9" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="I9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="M9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="N9" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="P9" t="s">
         <v>37</v>
@@ -1922,14 +1923,14 @@
         <v>45790</v>
       </c>
       <c r="D10" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="G10" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="I10" t="s">
         <v>47</v>
@@ -1941,16 +1942,16 @@
         <v>66147.5</v>
       </c>
       <c r="M10" t="s">
+        <v>59</v>
+      </c>
+      <c r="N10" t="s">
         <v>60</v>
       </c>
-      <c r="N10" t="s">
-        <v>61</v>
-      </c>
       <c r="O10" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="P10" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="Q10" t="s">
         <v>38</v>
@@ -1965,13 +1966,13 @@
         <v>90113131698</v>
       </c>
       <c r="AA10" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="AB10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="AC10" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.25">
@@ -1985,17 +1986,17 @@
         <v>45790</v>
       </c>
       <c r="D11" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" t="s">
+        <v>53</v>
+      </c>
+      <c r="G11" t="s">
         <v>54</v>
       </c>
-      <c r="G11" t="s">
+      <c r="I11" t="s">
         <v>55</v>
-      </c>
-      <c r="I11" t="s">
-        <v>56</v>
       </c>
       <c r="K11" s="2">
         <v>15000</v>
@@ -2024,14 +2025,14 @@
         <v>45790</v>
       </c>
       <c r="D12" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" t="s">
         <v>52</v>
       </c>
       <c r="G12" t="s">
-        <v>53</v>
+        <v>318</v>
       </c>
       <c r="I12" t="s">
         <v>41</v>
@@ -2040,7 +2041,7 @@
         <v>10000</v>
       </c>
       <c r="P12" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="V12" s="1">
         <v>45768</v>
@@ -2052,7 +2053,7 @@
         <v>36</v>
       </c>
       <c r="AC12" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.25">
@@ -2066,17 +2067,17 @@
         <v>45790</v>
       </c>
       <c r="D13" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="G13" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="I13" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="P13" t="s">
         <v>37</v>
@@ -2091,7 +2092,7 @@
         <v>36</v>
       </c>
       <c r="AC13" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.25">
@@ -2105,20 +2106,20 @@
         <v>45790</v>
       </c>
       <c r="D14" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="G14" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="I14" t="s">
         <v>41</v>
       </c>
       <c r="N14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P14" t="s">
         <v>37</v>
@@ -2133,7 +2134,7 @@
         <v>36</v>
       </c>
       <c r="AC14" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.25">
@@ -2147,26 +2148,26 @@
         <v>45790</v>
       </c>
       <c r="D15" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="G15" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="I15" t="s">
         <v>41</v>
       </c>
       <c r="M15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="N15" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="O15" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="P15" t="s">
         <v>37</v>
@@ -2181,13 +2182,13 @@
         <v>90113131698</v>
       </c>
       <c r="AA15" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="AB15" t="s">
         <v>36</v>
       </c>
       <c r="AC15" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.25">
@@ -2201,7 +2202,7 @@
         <v>45790</v>
       </c>
       <c r="D16" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" t="s">
@@ -2238,7 +2239,7 @@
         <v>36</v>
       </c>
       <c r="AC16" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
     </row>
     <row r="17" spans="1:30" x14ac:dyDescent="0.25">
@@ -2252,7 +2253,7 @@
         <v>45790</v>
       </c>
       <c r="D17" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" t="s">
@@ -2286,7 +2287,7 @@
         <v>36</v>
       </c>
       <c r="AC17" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
     </row>
     <row r="18" spans="1:30" x14ac:dyDescent="0.25">
@@ -2300,14 +2301,14 @@
         <v>45790</v>
       </c>
       <c r="D18" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="G18" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="I18" t="s">
         <v>47</v>
@@ -2319,19 +2320,19 @@
         <v>99000</v>
       </c>
       <c r="M18" t="s">
+        <v>59</v>
+      </c>
+      <c r="N18" t="s">
         <v>60</v>
       </c>
-      <c r="N18" t="s">
-        <v>61</v>
-      </c>
       <c r="O18" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="P18" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="Q18" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="V18" s="1">
         <v>45672</v>
@@ -2349,13 +2350,13 @@
         <v>45777</v>
       </c>
       <c r="AA18" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="AB18" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AC18" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
       <c r="AD18" s="1">
         <v>45777</v>
@@ -2372,7 +2373,7 @@
         <v>45790</v>
       </c>
       <c r="D19" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" t="s">
@@ -2397,7 +2398,7 @@
         <v>36</v>
       </c>
       <c r="AC19" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
     </row>
     <row r="20" spans="1:30" x14ac:dyDescent="0.25">
@@ -2411,14 +2412,14 @@
         <v>45790</v>
       </c>
       <c r="D20" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="G20" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="I20" t="s">
         <v>35</v>
@@ -2436,7 +2437,7 @@
         <v>36</v>
       </c>
       <c r="AC20" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
     </row>
     <row r="21" spans="1:30" x14ac:dyDescent="0.25">
@@ -2450,17 +2451,17 @@
         <v>45790</v>
       </c>
       <c r="D21" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="E21" s="1"/>
       <c r="F21" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="G21" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="I21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J21" s="2">
         <v>4561</v>
@@ -2469,13 +2470,13 @@
         <v>0</v>
       </c>
       <c r="M21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="N21" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="O21" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="P21" t="s">
         <v>37</v>
@@ -2490,13 +2491,13 @@
         <v>90113131698</v>
       </c>
       <c r="AA21" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="AB21" t="s">
         <v>36</v>
       </c>
       <c r="AC21" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
     </row>
     <row r="22" spans="1:30" x14ac:dyDescent="0.25">
@@ -2510,29 +2511,29 @@
         <v>45790</v>
       </c>
       <c r="D22" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="E22" s="1"/>
       <c r="F22" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="G22" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="I22" t="s">
         <v>31</v>
       </c>
       <c r="M22" t="s">
+        <v>59</v>
+      </c>
+      <c r="N22" t="s">
         <v>60</v>
       </c>
-      <c r="N22" t="s">
-        <v>61</v>
-      </c>
       <c r="O22" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="P22" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="Q22" t="s">
         <v>38</v>
@@ -2544,13 +2545,13 @@
         <v>90113131698</v>
       </c>
       <c r="AA22" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="AB22" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="AC22" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
     </row>
     <row r="23" spans="1:30" x14ac:dyDescent="0.25">
@@ -2564,29 +2565,29 @@
         <v>45790</v>
       </c>
       <c r="D23" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="G23" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="I23" t="s">
         <v>31</v>
       </c>
       <c r="M23" t="s">
+        <v>59</v>
+      </c>
+      <c r="N23" t="s">
         <v>60</v>
       </c>
-      <c r="N23" t="s">
-        <v>61</v>
-      </c>
       <c r="O23" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="P23" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="Q23" t="s">
         <v>38</v>
@@ -2598,13 +2599,13 @@
         <v>90113131698</v>
       </c>
       <c r="AA23" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="AB23" t="s">
         <v>36</v>
       </c>
       <c r="AC23" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
     </row>
     <row r="24" spans="1:30" x14ac:dyDescent="0.25">
@@ -2618,14 +2619,14 @@
         <v>45790</v>
       </c>
       <c r="D24" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="G24" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="I24" t="s">
         <v>41</v>
@@ -2637,13 +2638,13 @@
         <v>17974.900000000001</v>
       </c>
       <c r="M24" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="N24" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="O24" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="P24" t="s">
         <v>37</v>
@@ -2661,13 +2662,13 @@
         <v>90113131698</v>
       </c>
       <c r="AA24" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="AB24" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AC24" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
       <c r="AD24" s="1">
         <v>45740</v>
@@ -2684,23 +2685,23 @@
         <v>45790</v>
       </c>
       <c r="D25" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G25" t="s">
-        <v>63</v>
+        <v>323</v>
       </c>
       <c r="I25" t="s">
         <v>41</v>
       </c>
       <c r="M25" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="N25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P25" t="s">
         <v>37</v>
@@ -2715,7 +2716,7 @@
         <v>36</v>
       </c>
       <c r="AC25" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
     </row>
     <row r="26" spans="1:30" x14ac:dyDescent="0.25">
@@ -2729,29 +2730,29 @@
         <v>45790</v>
       </c>
       <c r="D26" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="E26" s="1"/>
       <c r="F26" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="G26" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="I26" t="s">
         <v>31</v>
       </c>
       <c r="M26" t="s">
+        <v>59</v>
+      </c>
+      <c r="N26" t="s">
         <v>60</v>
       </c>
-      <c r="N26" t="s">
-        <v>61</v>
-      </c>
       <c r="O26" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="P26" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="Q26" t="s">
         <v>38</v>
@@ -2766,13 +2767,13 @@
         <v>90113131698</v>
       </c>
       <c r="AA26" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="AB26" t="s">
         <v>36</v>
       </c>
       <c r="AC26" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
     </row>
     <row r="27" spans="1:30" x14ac:dyDescent="0.25">
@@ -2786,14 +2787,14 @@
         <v>45790</v>
       </c>
       <c r="D27" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="E27" s="1"/>
       <c r="F27" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="G27" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="I27" t="s">
         <v>47</v>
@@ -2808,16 +2809,16 @@
         <v>2500</v>
       </c>
       <c r="M27" t="s">
+        <v>59</v>
+      </c>
+      <c r="N27" t="s">
         <v>60</v>
       </c>
-      <c r="N27" t="s">
-        <v>61</v>
-      </c>
       <c r="O27" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="P27" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="Q27" t="s">
         <v>38</v>
@@ -2832,13 +2833,13 @@
         <v>90113131698</v>
       </c>
       <c r="AA27" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="AB27" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="AC27" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
     </row>
     <row r="28" spans="1:30" x14ac:dyDescent="0.25">
@@ -2852,14 +2853,14 @@
         <v>45790</v>
       </c>
       <c r="D28" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="E28" s="1"/>
       <c r="F28" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="G28" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="I28" t="s">
         <v>31</v>
@@ -2868,16 +2869,16 @@
         <v>5000</v>
       </c>
       <c r="M28" t="s">
+        <v>59</v>
+      </c>
+      <c r="N28" t="s">
         <v>60</v>
       </c>
-      <c r="N28" t="s">
-        <v>61</v>
-      </c>
       <c r="O28" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="P28" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="V28" s="1">
         <v>45664</v>
@@ -2886,13 +2887,13 @@
         <v>90113131698</v>
       </c>
       <c r="AA28" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="AB28" t="s">
         <v>36</v>
       </c>
       <c r="AC28" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
     </row>
     <row r="29" spans="1:30" x14ac:dyDescent="0.25">
@@ -2906,26 +2907,26 @@
         <v>45790</v>
       </c>
       <c r="D29" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="G29" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="I29" t="s">
+        <v>58</v>
+      </c>
+      <c r="M29" t="s">
         <v>59</v>
       </c>
-      <c r="M29" t="s">
+      <c r="N29" t="s">
         <v>60</v>
       </c>
-      <c r="N29" t="s">
-        <v>61</v>
-      </c>
       <c r="P29" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="V29" s="1">
         <v>45694</v>
@@ -2934,13 +2935,13 @@
         <v>90113131698</v>
       </c>
       <c r="AA29" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="AB29" t="s">
         <v>36</v>
       </c>
       <c r="AC29" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
     </row>
     <row r="30" spans="1:30" x14ac:dyDescent="0.25">
@@ -2954,14 +2955,14 @@
         <v>45790</v>
       </c>
       <c r="D30" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="E30" s="1"/>
       <c r="F30" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="G30" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="I30" t="s">
         <v>41</v>
@@ -2973,16 +2974,16 @@
         <v>7000</v>
       </c>
       <c r="M30" t="s">
+        <v>59</v>
+      </c>
+      <c r="N30" t="s">
         <v>60</v>
       </c>
-      <c r="N30" t="s">
-        <v>61</v>
-      </c>
       <c r="O30" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="P30" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="Q30" t="s">
         <v>38</v>
@@ -3000,13 +3001,13 @@
         <v>45777</v>
       </c>
       <c r="AA30" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="AB30" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="AC30" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
     </row>
     <row r="31" spans="1:30" x14ac:dyDescent="0.25">
@@ -3020,32 +3021,32 @@
         <v>45790</v>
       </c>
       <c r="D31" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="E31" s="1"/>
       <c r="F31" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="G31" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="I31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J31" s="2">
         <v>5000</v>
       </c>
       <c r="M31" t="s">
+        <v>59</v>
+      </c>
+      <c r="N31" t="s">
         <v>60</v>
       </c>
-      <c r="N31" t="s">
-        <v>61</v>
-      </c>
       <c r="O31" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="P31" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="Q31" t="s">
         <v>38</v>
@@ -3057,13 +3058,13 @@
         <v>90113131698</v>
       </c>
       <c r="AA31" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="AB31" t="s">
         <v>36</v>
       </c>
       <c r="AC31" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
     </row>
     <row r="32" spans="1:30" x14ac:dyDescent="0.25">
@@ -3077,14 +3078,14 @@
         <v>45790</v>
       </c>
       <c r="D32" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="E32" s="1"/>
       <c r="F32" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="G32" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="I32" t="s">
         <v>31</v>
@@ -3096,19 +3097,19 @@
         <v>25000</v>
       </c>
       <c r="M32" t="s">
+        <v>59</v>
+      </c>
+      <c r="N32" t="s">
         <v>60</v>
       </c>
-      <c r="N32" t="s">
-        <v>61</v>
-      </c>
       <c r="O32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="P32" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="Q32" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="V32" s="1">
         <v>45664</v>
@@ -3123,13 +3124,13 @@
         <v>90113131698</v>
       </c>
       <c r="AA32" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="AB32" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="AC32" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
     </row>
     <row r="33" spans="1:30" x14ac:dyDescent="0.25">
@@ -3143,14 +3144,14 @@
         <v>45790</v>
       </c>
       <c r="D33" t="s">
-        <v>307</v>
+        <v>300</v>
       </c>
       <c r="E33" s="1"/>
       <c r="F33" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="G33" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="I33" t="s">
         <v>31</v>
@@ -3159,16 +3160,16 @@
         <v>5000</v>
       </c>
       <c r="M33" t="s">
+        <v>59</v>
+      </c>
+      <c r="N33" t="s">
         <v>60</v>
       </c>
-      <c r="N33" t="s">
-        <v>61</v>
-      </c>
       <c r="O33" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="P33" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="V33" s="1">
         <v>45664</v>
@@ -3177,13 +3178,13 @@
         <v>90113131698</v>
       </c>
       <c r="AA33" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="AB33" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="AC33" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
     </row>
     <row r="34" spans="1:30" x14ac:dyDescent="0.25">
@@ -3197,17 +3198,17 @@
         <v>45790</v>
       </c>
       <c r="D34" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
       <c r="E34" s="1"/>
       <c r="F34" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="G34" t="s">
-        <v>228</v>
+        <v>319</v>
       </c>
       <c r="I34" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="J34" s="2">
         <v>5000</v>
@@ -3216,19 +3217,19 @@
         <v>10000</v>
       </c>
       <c r="M34" t="s">
+        <v>59</v>
+      </c>
+      <c r="N34" t="s">
         <v>60</v>
       </c>
-      <c r="N34" t="s">
-        <v>61</v>
-      </c>
       <c r="O34" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="P34" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="Q34" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="V34" s="1">
         <v>45662</v>
@@ -3246,10 +3247,10 @@
         <v>32</v>
       </c>
       <c r="AB34" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="AC34" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
     </row>
     <row r="35" spans="1:30" x14ac:dyDescent="0.25">
@@ -3263,7 +3264,7 @@
         <v>45790</v>
       </c>
       <c r="D35" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="E35" s="1"/>
       <c r="F35" t="s">
@@ -3285,13 +3286,13 @@
         <v>0</v>
       </c>
       <c r="M35" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="O35" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="P35" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="V35" s="1">
         <v>45715</v>
@@ -3303,10 +3304,10 @@
         <v>32</v>
       </c>
       <c r="AB35" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="AC35" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
     </row>
     <row r="36" spans="1:30" x14ac:dyDescent="0.25">
@@ -3320,14 +3321,14 @@
         <v>45790</v>
       </c>
       <c r="D36" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="E36" s="1"/>
       <c r="F36" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="G36" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="I36" t="s">
         <v>31</v>
@@ -3336,16 +3337,16 @@
         <v>1800</v>
       </c>
       <c r="M36" t="s">
+        <v>59</v>
+      </c>
+      <c r="N36" t="s">
         <v>60</v>
       </c>
-      <c r="N36" t="s">
-        <v>61</v>
-      </c>
       <c r="O36" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="P36" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="Q36" t="s">
         <v>38</v>
@@ -3360,10 +3361,10 @@
         <v>32</v>
       </c>
       <c r="AB36" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AC36" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="AD36" s="1">
         <v>45740</v>
@@ -3380,14 +3381,14 @@
         <v>45790</v>
       </c>
       <c r="D37" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="E37" s="1"/>
       <c r="F37" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G37" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="I37" t="s">
         <v>31</v>
@@ -3396,16 +3397,16 @@
         <v>5000</v>
       </c>
       <c r="M37" t="s">
+        <v>59</v>
+      </c>
+      <c r="N37" t="s">
         <v>60</v>
       </c>
-      <c r="N37" t="s">
-        <v>61</v>
-      </c>
       <c r="O37" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="P37" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="V37" s="1">
         <v>45716</v>
@@ -3417,13 +3418,13 @@
         <v>90113131698</v>
       </c>
       <c r="AA37" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="AB37" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="AC37" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
     </row>
     <row r="38" spans="1:30" x14ac:dyDescent="0.25">
@@ -3437,29 +3438,29 @@
         <v>45790</v>
       </c>
       <c r="D38" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
       <c r="E38" s="1"/>
       <c r="F38" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="G38" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="I38" t="s">
         <v>31</v>
       </c>
       <c r="M38" t="s">
+        <v>59</v>
+      </c>
+      <c r="N38" t="s">
         <v>60</v>
       </c>
-      <c r="N38" t="s">
-        <v>61</v>
-      </c>
       <c r="O38" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="P38" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="Q38" t="s">
         <v>38</v>
@@ -3474,13 +3475,13 @@
         <v>90113131698</v>
       </c>
       <c r="AA38" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="AB38" t="s">
         <v>36</v>
       </c>
       <c r="AC38" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
     </row>
     <row r="39" spans="1:30" x14ac:dyDescent="0.25">
@@ -3494,14 +3495,14 @@
         <v>45790</v>
       </c>
       <c r="D39" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
       <c r="E39" s="1"/>
       <c r="F39" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="G39" t="s">
-        <v>198</v>
+        <v>320</v>
       </c>
       <c r="I39" t="s">
         <v>31</v>
@@ -3510,13 +3511,13 @@
         <v>17890</v>
       </c>
       <c r="M39" t="s">
+        <v>59</v>
+      </c>
+      <c r="N39" t="s">
         <v>60</v>
       </c>
-      <c r="N39" t="s">
-        <v>61</v>
-      </c>
       <c r="O39" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="P39" t="s">
         <v>37</v>
@@ -3531,13 +3532,13 @@
         <v>45820</v>
       </c>
       <c r="AA39" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="AB39" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="AC39" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
     </row>
     <row r="40" spans="1:30" x14ac:dyDescent="0.25">
@@ -3551,26 +3552,26 @@
         <v>45790</v>
       </c>
       <c r="D40" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="E40" s="1"/>
       <c r="F40" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="G40" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="I40" t="s">
         <v>41</v>
       </c>
       <c r="M40" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="N40" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="O40" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="P40" t="s">
         <v>37</v>
@@ -3585,13 +3586,13 @@
         <v>90113131698</v>
       </c>
       <c r="AA40" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="AB40" t="s">
         <v>36</v>
       </c>
       <c r="AC40" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
     </row>
     <row r="41" spans="1:30" x14ac:dyDescent="0.25">
@@ -3605,14 +3606,14 @@
         <v>45790</v>
       </c>
       <c r="D41" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="E41" s="1"/>
       <c r="F41" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="G41" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="I41" t="s">
         <v>31</v>
@@ -3624,16 +3625,16 @@
         <v>16416</v>
       </c>
       <c r="M41" t="s">
+        <v>59</v>
+      </c>
+      <c r="N41" t="s">
         <v>60</v>
       </c>
-      <c r="N41" t="s">
-        <v>61</v>
-      </c>
       <c r="O41" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="P41" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="V41" s="1">
         <v>45715</v>
@@ -3648,13 +3649,13 @@
         <v>45799</v>
       </c>
       <c r="AA41" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AB41" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="AC41" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
     </row>
     <row r="42" spans="1:30" x14ac:dyDescent="0.25">
@@ -3668,14 +3669,14 @@
         <v>45790</v>
       </c>
       <c r="D42" t="s">
-        <v>311</v>
+        <v>304</v>
       </c>
       <c r="E42" s="1"/>
       <c r="F42" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="G42" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="I42" t="s">
         <v>31</v>
@@ -3687,19 +3688,19 @@
         <v>37618.769999999997</v>
       </c>
       <c r="M42" t="s">
+        <v>59</v>
+      </c>
+      <c r="N42" t="s">
         <v>60</v>
       </c>
-      <c r="N42" t="s">
-        <v>61</v>
-      </c>
       <c r="O42" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="P42" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="Q42" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="V42" s="1">
         <v>45662</v>
@@ -3711,13 +3712,13 @@
         <v>90113131698</v>
       </c>
       <c r="AA42" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="AB42" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AC42" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="AD42" s="1">
         <v>45740</v>
@@ -3734,17 +3735,17 @@
         <v>45790</v>
       </c>
       <c r="D43" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="E43" s="1"/>
       <c r="F43" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="G43" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="I43" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="P43" t="s">
         <v>37</v>
@@ -3759,7 +3760,7 @@
         <v>36</v>
       </c>
       <c r="AC43" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
     </row>
     <row r="44" spans="1:30" x14ac:dyDescent="0.25">
@@ -3773,29 +3774,29 @@
         <v>45790</v>
       </c>
       <c r="D44" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="E44" s="1"/>
       <c r="F44" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="G44" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="I44" t="s">
         <v>47</v>
       </c>
       <c r="M44" t="s">
+        <v>59</v>
+      </c>
+      <c r="N44" t="s">
         <v>60</v>
       </c>
-      <c r="N44" t="s">
-        <v>61</v>
-      </c>
       <c r="O44" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="P44" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="Q44" t="s">
         <v>38</v>
@@ -3810,13 +3811,13 @@
         <v>90113131698</v>
       </c>
       <c r="AA44" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="AB44" t="s">
         <v>36</v>
       </c>
       <c r="AC44" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
     </row>
     <row r="45" spans="1:30" x14ac:dyDescent="0.25">
@@ -3830,32 +3831,32 @@
         <v>45790</v>
       </c>
       <c r="D45" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="E45" s="1"/>
       <c r="F45" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="G45" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="I45" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J45" s="2">
         <v>5000</v>
       </c>
       <c r="M45" t="s">
+        <v>59</v>
+      </c>
+      <c r="N45" t="s">
         <v>60</v>
       </c>
-      <c r="N45" t="s">
-        <v>61</v>
-      </c>
       <c r="O45" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="P45" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="V45" s="1">
         <v>45701</v>
@@ -3864,13 +3865,13 @@
         <v>90113131698</v>
       </c>
       <c r="AA45" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="AB45" t="s">
         <v>36</v>
       </c>
       <c r="AC45" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
     </row>
     <row r="46" spans="1:30" x14ac:dyDescent="0.25">
@@ -3884,29 +3885,29 @@
         <v>45790</v>
       </c>
       <c r="D46" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="E46" s="1"/>
       <c r="F46" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="G46" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I46" t="s">
         <v>41</v>
       </c>
       <c r="M46" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="N46" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="O46" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="P46" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="V46" s="1">
         <v>45716</v>
@@ -3918,13 +3919,13 @@
         <v>90113131698</v>
       </c>
       <c r="AA46" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="AB46" t="s">
         <v>36</v>
       </c>
       <c r="AC46" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
     </row>
     <row r="47" spans="1:30" x14ac:dyDescent="0.25">
@@ -3938,17 +3939,17 @@
         <v>45790</v>
       </c>
       <c r="D47" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="E47" s="1"/>
       <c r="F47" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G47" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I47" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J47" s="2">
         <v>10557</v>
@@ -3957,13 +3958,13 @@
         <v>10500</v>
       </c>
       <c r="M47" t="s">
+        <v>59</v>
+      </c>
+      <c r="N47" t="s">
         <v>60</v>
       </c>
-      <c r="N47" t="s">
-        <v>61</v>
-      </c>
       <c r="P47" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="V47" s="1">
         <v>45716</v>
@@ -3975,13 +3976,13 @@
         <v>90113131698</v>
       </c>
       <c r="AA47" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="AB47" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="AC47" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
     </row>
     <row r="48" spans="1:30" x14ac:dyDescent="0.25">
@@ -3995,29 +3996,29 @@
         <v>45790</v>
       </c>
       <c r="D48" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="E48" s="1"/>
       <c r="F48" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="G48" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="I48" t="s">
         <v>41</v>
       </c>
       <c r="M48" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="N48" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="O48" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="P48" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="V48" s="1">
         <v>45716</v>
@@ -4029,13 +4030,13 @@
         <v>90113131698</v>
       </c>
       <c r="AA48" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="AB48" t="s">
         <v>36</v>
       </c>
       <c r="AC48" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
     </row>
     <row r="49" spans="1:30" x14ac:dyDescent="0.25">
@@ -4049,23 +4050,23 @@
         <v>45790</v>
       </c>
       <c r="D49" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="E49" s="1"/>
       <c r="F49" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="G49" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="I49" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="M49" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="N49" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="P49" t="s">
         <v>37</v>
@@ -4091,7 +4092,7 @@
         <v>45790</v>
       </c>
       <c r="D50" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="E50" s="1"/>
       <c r="F50" t="s">
@@ -4113,7 +4114,7 @@
         <v>36</v>
       </c>
       <c r="AC50" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
     </row>
     <row r="51" spans="1:30" x14ac:dyDescent="0.25">
@@ -4127,14 +4128,14 @@
         <v>45790</v>
       </c>
       <c r="D51" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
       <c r="E51" s="1"/>
       <c r="F51" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="G51" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="I51" t="s">
         <v>31</v>
@@ -4143,19 +4144,19 @@
         <v>5000</v>
       </c>
       <c r="M51" t="s">
+        <v>59</v>
+      </c>
+      <c r="N51" t="s">
         <v>60</v>
       </c>
-      <c r="N51" t="s">
-        <v>61</v>
-      </c>
       <c r="O51" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="P51" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="Q51" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="V51" s="1">
         <v>45664</v>
@@ -4167,13 +4168,13 @@
         <v>90113131698</v>
       </c>
       <c r="AA51" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AB51" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="AC51" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
     </row>
     <row r="52" spans="1:30" x14ac:dyDescent="0.25">
@@ -4187,29 +4188,29 @@
         <v>45790</v>
       </c>
       <c r="D52" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="E52" s="1"/>
       <c r="F52" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="G52" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="I52" t="s">
         <v>31</v>
       </c>
       <c r="M52" t="s">
+        <v>59</v>
+      </c>
+      <c r="N52" t="s">
         <v>60</v>
       </c>
-      <c r="N52" t="s">
-        <v>61</v>
-      </c>
       <c r="O52" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="P52" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="Q52" t="s">
         <v>38</v>
@@ -4224,13 +4225,13 @@
         <v>90113131698</v>
       </c>
       <c r="AA52" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="AB52" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="AC52" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
     </row>
     <row r="53" spans="1:30" x14ac:dyDescent="0.25">
@@ -4244,17 +4245,17 @@
         <v>45790</v>
       </c>
       <c r="D53" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
       <c r="E53" s="1"/>
       <c r="F53" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="G53" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="I53" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J53" s="2">
         <v>2500</v>
@@ -4263,19 +4264,19 @@
         <v>180000</v>
       </c>
       <c r="M53" t="s">
+        <v>59</v>
+      </c>
+      <c r="N53" t="s">
         <v>60</v>
       </c>
-      <c r="N53" t="s">
-        <v>61</v>
-      </c>
       <c r="O53" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="P53" t="s">
         <v>37</v>
       </c>
       <c r="Q53" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="V53" s="1">
         <v>45701</v>
@@ -4287,13 +4288,13 @@
         <v>90113131698</v>
       </c>
       <c r="AA53" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="AB53" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="AC53" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
     </row>
     <row r="54" spans="1:30" x14ac:dyDescent="0.25">
@@ -4307,14 +4308,14 @@
         <v>45790</v>
       </c>
       <c r="D54" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="E54" s="1"/>
       <c r="F54" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="G54" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="I54" t="s">
         <v>31</v>
@@ -4326,13 +4327,13 @@
         <v>9286</v>
       </c>
       <c r="M54" t="s">
+        <v>59</v>
+      </c>
+      <c r="N54" t="s">
         <v>60</v>
       </c>
-      <c r="N54" t="s">
-        <v>61</v>
-      </c>
       <c r="O54" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="P54" t="s">
         <v>37</v>
@@ -4353,13 +4354,13 @@
         <v>45789</v>
       </c>
       <c r="AA54" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="AB54" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="AC54" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
     </row>
     <row r="55" spans="1:30" x14ac:dyDescent="0.25">
@@ -4373,14 +4374,14 @@
         <v>45790</v>
       </c>
       <c r="D55" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="E55" s="1"/>
       <c r="F55" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="G55" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="I55" t="s">
         <v>31</v>
@@ -4392,19 +4393,19 @@
         <v>28594</v>
       </c>
       <c r="M55" t="s">
+        <v>59</v>
+      </c>
+      <c r="N55" t="s">
         <v>60</v>
       </c>
-      <c r="N55" t="s">
-        <v>61</v>
-      </c>
       <c r="O55" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="P55" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="Q55" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="V55" s="1">
         <v>45662</v>
@@ -4416,13 +4417,13 @@
         <v>90113131698</v>
       </c>
       <c r="AA55" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="AB55" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AC55" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="AD55" s="1">
         <v>45740</v>
@@ -4439,17 +4440,17 @@
         <v>45790</v>
       </c>
       <c r="D56" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="E56" s="1"/>
       <c r="F56" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="G56" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="I56" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="P56" t="s">
         <v>37</v>
@@ -4464,7 +4465,7 @@
         <v>36</v>
       </c>
       <c r="AC56" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
     </row>
     <row r="57" spans="1:30" x14ac:dyDescent="0.25">
@@ -4478,17 +4479,17 @@
         <v>45790</v>
       </c>
       <c r="D57" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="E57" s="1"/>
       <c r="F57" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G57" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I57" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="P57" t="s">
         <v>37</v>
@@ -4503,7 +4504,7 @@
         <v>36</v>
       </c>
       <c r="AC57" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
     </row>
     <row r="58" spans="1:30" x14ac:dyDescent="0.25">
@@ -4517,26 +4518,26 @@
         <v>45790</v>
       </c>
       <c r="D58" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="E58" s="1"/>
       <c r="F58" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G58" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="I58" t="s">
         <v>41</v>
       </c>
       <c r="M58" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="N58" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="O58" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="P58" t="s">
         <v>37</v>
@@ -4554,13 +4555,13 @@
         <v>90113131698</v>
       </c>
       <c r="AA58" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="AB58" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AC58" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
       <c r="AD58" s="1">
         <v>45740</v>
@@ -4577,26 +4578,26 @@
         <v>45790</v>
       </c>
       <c r="D59" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="E59" s="1"/>
       <c r="F59" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="G59" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="I59" t="s">
+        <v>58</v>
+      </c>
+      <c r="M59" t="s">
         <v>59</v>
       </c>
-      <c r="M59" t="s">
+      <c r="N59" t="s">
         <v>60</v>
       </c>
-      <c r="N59" t="s">
-        <v>61</v>
-      </c>
       <c r="P59" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="V59" s="1">
         <v>45701</v>
@@ -4605,13 +4606,13 @@
         <v>90113131698</v>
       </c>
       <c r="AA59" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="AB59" t="s">
         <v>36</v>
       </c>
       <c r="AC59" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
     </row>
     <row r="60" spans="1:30" x14ac:dyDescent="0.25">
@@ -4625,26 +4626,26 @@
         <v>45790</v>
       </c>
       <c r="D60" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="E60" s="1"/>
       <c r="F60" t="s">
+        <v>56</v>
+      </c>
+      <c r="G60" t="s">
         <v>57</v>
       </c>
-      <c r="G60" t="s">
+      <c r="I60" t="s">
         <v>58</v>
       </c>
-      <c r="I60" t="s">
+      <c r="M60" t="s">
         <v>59</v>
       </c>
-      <c r="M60" t="s">
+      <c r="N60" t="s">
         <v>60</v>
       </c>
-      <c r="N60" t="s">
-        <v>61</v>
-      </c>
       <c r="P60" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="V60" s="1">
         <v>45761</v>
@@ -4656,7 +4657,7 @@
         <v>36</v>
       </c>
       <c r="AC60" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
     </row>
     <row r="61" spans="1:30" x14ac:dyDescent="0.25">
@@ -4670,7 +4671,7 @@
         <v>45790</v>
       </c>
       <c r="D61" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E61" s="1"/>
       <c r="F61" t="s">
@@ -4686,7 +4687,7 @@
         <v>10000</v>
       </c>
       <c r="P61" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="V61" s="1">
         <v>45768</v>
@@ -4698,7 +4699,7 @@
         <v>36</v>
       </c>
       <c r="AC61" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
     </row>
     <row r="62" spans="1:30" x14ac:dyDescent="0.25">
@@ -4712,29 +4713,29 @@
         <v>45790</v>
       </c>
       <c r="D62" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="E62" s="1"/>
       <c r="F62" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="G62" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="I62" t="s">
         <v>47</v>
       </c>
       <c r="M62" t="s">
+        <v>59</v>
+      </c>
+      <c r="N62" t="s">
         <v>60</v>
       </c>
-      <c r="N62" t="s">
-        <v>61</v>
-      </c>
       <c r="O62" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="P62" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="V62" s="1">
         <v>45712</v>
@@ -4746,13 +4747,13 @@
         <v>90113131698</v>
       </c>
       <c r="AA62" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="AB62" t="s">
         <v>36</v>
       </c>
       <c r="AC62" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
     </row>
     <row r="63" spans="1:30" x14ac:dyDescent="0.25">
@@ -4766,14 +4767,14 @@
         <v>45790</v>
       </c>
       <c r="D63" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="E63" s="1"/>
       <c r="F63" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="G63" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="I63" t="s">
         <v>41</v>
@@ -4788,13 +4789,13 @@
         <v>8000</v>
       </c>
       <c r="M63" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="O63" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="P63" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="V63" s="1">
         <v>45716</v>
@@ -4806,13 +4807,13 @@
         <v>90113131698</v>
       </c>
       <c r="AA63" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="AB63" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="AC63" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
     </row>
     <row r="64" spans="1:30" x14ac:dyDescent="0.25">
@@ -4826,32 +4827,32 @@
         <v>45790</v>
       </c>
       <c r="D64" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="E64" s="1"/>
       <c r="F64" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="G64" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="I64" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="L64" s="2">
         <v>7500</v>
       </c>
       <c r="M64" t="s">
+        <v>59</v>
+      </c>
+      <c r="N64" t="s">
         <v>60</v>
       </c>
-      <c r="N64" t="s">
-        <v>61</v>
-      </c>
       <c r="O64" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="P64" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="Q64" t="s">
         <v>38</v>
@@ -4863,10 +4864,10 @@
         <v>90113131698</v>
       </c>
       <c r="AA64" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="AB64" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AD64" s="1">
         <v>45740</v>
@@ -4883,17 +4884,17 @@
         <v>45790</v>
       </c>
       <c r="D65" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="E65" s="1"/>
       <c r="F65" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G65" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="I65" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J65" s="2">
         <v>4000</v>
@@ -4905,7 +4906,7 @@
         <v>20000</v>
       </c>
       <c r="P65" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="V65" s="1">
         <v>45747</v>
@@ -4914,13 +4915,13 @@
         <v>90113131698</v>
       </c>
       <c r="AA65" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="AB65" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="AC65" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
     </row>
     <row r="66" spans="1:29" x14ac:dyDescent="0.25">
@@ -4934,23 +4935,23 @@
         <v>45790</v>
       </c>
       <c r="D66" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="E66" s="1"/>
       <c r="F66" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="G66" t="s">
-        <v>168</v>
+        <v>321</v>
       </c>
       <c r="I66" t="s">
         <v>41</v>
       </c>
       <c r="M66" t="s">
+        <v>59</v>
+      </c>
+      <c r="N66" t="s">
         <v>60</v>
-      </c>
-      <c r="N66" t="s">
-        <v>61</v>
       </c>
       <c r="P66" t="s">
         <v>37</v>
@@ -4965,7 +4966,7 @@
         <v>36</v>
       </c>
       <c r="AC66" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
     </row>
     <row r="67" spans="1:29" x14ac:dyDescent="0.25">
@@ -4979,32 +4980,32 @@
         <v>45790</v>
       </c>
       <c r="D67" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
       <c r="E67" s="1"/>
       <c r="F67" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="G67" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="I67" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J67" s="2">
         <v>5000</v>
       </c>
       <c r="M67" t="s">
+        <v>59</v>
+      </c>
+      <c r="N67" t="s">
         <v>60</v>
       </c>
-      <c r="N67" t="s">
-        <v>61</v>
-      </c>
       <c r="O67" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="P67" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="Q67" t="s">
         <v>38</v>
@@ -5016,13 +5017,13 @@
         <v>90113131698</v>
       </c>
       <c r="AA67" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="AB67" t="s">
         <v>36</v>
       </c>
       <c r="AC67" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
     </row>
     <row r="68" spans="1:29" x14ac:dyDescent="0.25">
@@ -5036,14 +5037,14 @@
         <v>45790</v>
       </c>
       <c r="D68" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="E68" s="1"/>
       <c r="F68" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="G68" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="I68" t="s">
         <v>31</v>
@@ -5055,19 +5056,19 @@
         <v>3434</v>
       </c>
       <c r="M68" t="s">
+        <v>59</v>
+      </c>
+      <c r="N68" t="s">
         <v>60</v>
       </c>
-      <c r="N68" t="s">
-        <v>61</v>
-      </c>
       <c r="O68" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="P68" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="Q68" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="V68" s="1">
         <v>45662</v>
@@ -5079,13 +5080,13 @@
         <v>90113131698</v>
       </c>
       <c r="AA68" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="AB68" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="AC68" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
     </row>
     <row r="69" spans="1:29" x14ac:dyDescent="0.25">
@@ -5099,17 +5100,17 @@
         <v>45790</v>
       </c>
       <c r="D69" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="E69" s="1"/>
       <c r="F69" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G69" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="I69" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="P69" t="s">
         <v>37</v>
@@ -5124,7 +5125,7 @@
         <v>36</v>
       </c>
       <c r="AC69" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
     </row>
     <row r="70" spans="1:29" x14ac:dyDescent="0.25">
@@ -5138,14 +5139,14 @@
         <v>45790</v>
       </c>
       <c r="D70" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="E70" s="1"/>
       <c r="F70" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="G70" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="I70" t="s">
         <v>31</v>
@@ -5154,19 +5155,19 @@
         <v>14000</v>
       </c>
       <c r="M70" t="s">
+        <v>59</v>
+      </c>
+      <c r="N70" t="s">
         <v>60</v>
       </c>
-      <c r="N70" t="s">
-        <v>61</v>
-      </c>
       <c r="O70" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="P70" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="Q70" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="V70" s="1">
         <v>45715</v>
@@ -5178,13 +5179,13 @@
         <v>45791</v>
       </c>
       <c r="AA70" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="AB70" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="AC70" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
     </row>
     <row r="71" spans="1:29" x14ac:dyDescent="0.25">
@@ -5198,7 +5199,7 @@
         <v>45790</v>
       </c>
       <c r="D71" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="E71" s="1"/>
       <c r="F71" t="s">
@@ -5220,7 +5221,7 @@
         <v>36</v>
       </c>
       <c r="AC71" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
     </row>
     <row r="72" spans="1:29" x14ac:dyDescent="0.25">
@@ -5234,14 +5235,14 @@
         <v>45790</v>
       </c>
       <c r="D72" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="E72" s="1"/>
       <c r="F72" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="G72" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="I72" t="s">
         <v>31</v>
@@ -5253,16 +5254,16 @@
         <v>28400</v>
       </c>
       <c r="M72" t="s">
+        <v>59</v>
+      </c>
+      <c r="N72" t="s">
         <v>60</v>
       </c>
-      <c r="N72" t="s">
-        <v>61</v>
-      </c>
       <c r="O72" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="P72" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="V72" s="1">
         <v>45715</v>
@@ -5274,13 +5275,13 @@
         <v>45812</v>
       </c>
       <c r="AA72" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="AB72" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="AC72" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
     </row>
     <row r="73" spans="1:29" x14ac:dyDescent="0.25">
@@ -5294,14 +5295,14 @@
         <v>45790</v>
       </c>
       <c r="D73" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="E73" s="1"/>
       <c r="F73" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="G73" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="I73" t="s">
         <v>31</v>
@@ -5310,16 +5311,16 @@
         <v>1800</v>
       </c>
       <c r="M73" t="s">
+        <v>59</v>
+      </c>
+      <c r="N73" t="s">
         <v>60</v>
       </c>
-      <c r="N73" t="s">
-        <v>61</v>
-      </c>
       <c r="O73" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="P73" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="V73" s="1">
         <v>45747</v>
@@ -5331,13 +5332,13 @@
         <v>45786</v>
       </c>
       <c r="AA73" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="AB73" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="AC73" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
     </row>
     <row r="74" spans="1:29" x14ac:dyDescent="0.25">
@@ -5351,14 +5352,14 @@
         <v>45790</v>
       </c>
       <c r="D74" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="E74" s="1"/>
       <c r="F74" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="G74" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="I74" t="s">
         <v>31</v>
@@ -5370,16 +5371,16 @@
         <v>10000</v>
       </c>
       <c r="M74" t="s">
+        <v>59</v>
+      </c>
+      <c r="N74" t="s">
         <v>60</v>
       </c>
-      <c r="N74" t="s">
-        <v>61</v>
-      </c>
       <c r="O74" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="P74" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="V74" s="1">
         <v>45716</v>
@@ -5391,13 +5392,13 @@
         <v>45785</v>
       </c>
       <c r="AA74" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="AB74" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="AC74" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
     </row>
     <row r="75" spans="1:29" x14ac:dyDescent="0.25">
@@ -5411,14 +5412,14 @@
         <v>45790</v>
       </c>
       <c r="D75" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="E75" s="1"/>
       <c r="F75" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="G75" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="I75" t="s">
         <v>31</v>
@@ -5427,19 +5428,19 @@
         <v>5000</v>
       </c>
       <c r="M75" t="s">
+        <v>59</v>
+      </c>
+      <c r="N75" t="s">
         <v>60</v>
       </c>
-      <c r="N75" t="s">
-        <v>61</v>
-      </c>
       <c r="O75" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="P75" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="Q75" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="V75" s="1">
         <v>45715</v>
@@ -5454,13 +5455,13 @@
         <v>45782</v>
       </c>
       <c r="AA75" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="AB75" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="AC75" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
     </row>
     <row r="76" spans="1:29" x14ac:dyDescent="0.25">
@@ -5474,14 +5475,14 @@
         <v>45790</v>
       </c>
       <c r="D76" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="E76" s="1"/>
       <c r="F76" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="G76" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="I76" t="s">
         <v>31</v>
@@ -5493,19 +5494,19 @@
         <v>40000</v>
       </c>
       <c r="M76" t="s">
+        <v>59</v>
+      </c>
+      <c r="N76" t="s">
         <v>60</v>
       </c>
-      <c r="N76" t="s">
-        <v>61</v>
-      </c>
       <c r="O76" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="P76" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="Q76" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="V76" s="1">
         <v>45716</v>
@@ -5520,13 +5521,13 @@
         <v>45792</v>
       </c>
       <c r="AA76" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="AB76" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="AC76" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
     </row>
     <row r="77" spans="1:29" x14ac:dyDescent="0.25">
@@ -5540,29 +5541,29 @@
         <v>45790</v>
       </c>
       <c r="D77" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="E77" s="1"/>
       <c r="F77" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="G77" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="I77" t="s">
         <v>41</v>
       </c>
       <c r="M77" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="N77" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="O77" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="P77" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="V77" s="1">
         <v>45694</v>
@@ -5571,13 +5572,13 @@
         <v>90113131698</v>
       </c>
       <c r="AA77" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="AB77" t="s">
         <v>36</v>
       </c>
       <c r="AC77" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
     </row>
     <row r="78" spans="1:29" x14ac:dyDescent="0.25">
@@ -5591,14 +5592,14 @@
         <v>45790</v>
       </c>
       <c r="D78" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="E78" s="1"/>
       <c r="F78" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="G78" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="I78" t="s">
         <v>31</v>
@@ -5607,13 +5608,13 @@
         <v>21802</v>
       </c>
       <c r="M78" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="N78" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="O78" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="P78" t="s">
         <v>37</v>
@@ -5634,13 +5635,13 @@
         <v>45777</v>
       </c>
       <c r="AA78" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="AB78" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="AC78" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
     </row>
     <row r="79" spans="1:29" x14ac:dyDescent="0.25">
@@ -5654,14 +5655,14 @@
         <v>45790</v>
       </c>
       <c r="D79" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="E79" s="1"/>
       <c r="F79" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="G79" t="s">
-        <v>194</v>
+        <v>322</v>
       </c>
       <c r="I79" t="s">
         <v>31</v>
@@ -5673,19 +5674,19 @@
         <v>5000</v>
       </c>
       <c r="M79" t="s">
+        <v>59</v>
+      </c>
+      <c r="N79" t="s">
         <v>60</v>
       </c>
-      <c r="N79" t="s">
-        <v>61</v>
-      </c>
       <c r="O79" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="P79" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="Q79" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="V79" s="1">
         <v>45756</v>
@@ -5703,13 +5704,13 @@
         <v>45806</v>
       </c>
       <c r="AA79" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="AB79" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="AC79" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
     </row>
     <row r="80" spans="1:29" x14ac:dyDescent="0.25">
@@ -5723,23 +5724,23 @@
         <v>45790</v>
       </c>
       <c r="D80" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="E80" s="1"/>
       <c r="F80" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="G80" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="I80" t="s">
         <v>41</v>
       </c>
       <c r="M80" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="N80" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="P80" t="s">
         <v>37</v>
@@ -5754,7 +5755,7 @@
         <v>36</v>
       </c>
       <c r="AC80" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
     </row>
     <row r="81" spans="1:29" x14ac:dyDescent="0.25">
@@ -5768,26 +5769,26 @@
         <v>45790</v>
       </c>
       <c r="D81" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
       <c r="E81" s="1"/>
       <c r="F81" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="G81" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="I81" t="s">
         <v>31</v>
       </c>
       <c r="M81" t="s">
+        <v>59</v>
+      </c>
+      <c r="N81" t="s">
         <v>60</v>
       </c>
-      <c r="N81" t="s">
-        <v>61</v>
-      </c>
       <c r="P81" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="V81" s="1">
         <v>45664</v>
@@ -5796,13 +5797,13 @@
         <v>90113131698</v>
       </c>
       <c r="AA81" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="AB81" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="AC81" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
     </row>
   </sheetData>

</xml_diff>